<commit_message>
Added ERD to document and created project for website
</commit_message>
<xml_diff>
--- a/Normalisation.xlsx
+++ b/Normalisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\ISAD251CW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6348830-FBCC-407F-A8FC-E1EF0177C770}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CEC6DA0-CD95-4A9F-84F8-B07B13DE921A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BFD22851-2DF0-4298-A0AB-6354F9255377}"/>
   </bookViews>
@@ -484,7 +484,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated the SQL and database
</commit_message>
<xml_diff>
--- a/Normalisation.xlsx
+++ b/Normalisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\ISAD251CW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CEC6DA0-CD95-4A9F-84F8-B07B13DE921A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFB5E44-3EF8-46F5-93B2-89782A3219AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BFD22851-2DF0-4298-A0AB-6354F9255377}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>UNF</t>
   </si>
@@ -481,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0744E9-C34C-4C84-A678-9B44716B3931}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,44 +621,39 @@
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
         <v>23</v>
       </c>
     </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" t="s">
-        <v>28</v>
+      <c r="D20" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D21" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D22" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D23" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D24" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D25" s="2" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>